<commit_message>
add socketTimeOut properties for mysql connection
</commit_message>
<xml_diff>
--- a/src/test/resources/io.dingodb.test/testdata/btreemysqlcases/prepareStatement/mysql_ps_batch_cases_btree.xlsx
+++ b/src/test/resources/io.dingodb.test/testdata/btreemysqlcases/prepareStatement/mysql_ps_batch_cases_btree.xlsx
@@ -141,26 +141,26 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>20000</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>select count(*) from $schema26 where id&gt;4000 and id&lt;=20000</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>16000</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>update $schema26 set name='BJ' where id&gt;4000 and id&lt;=20000</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>y</t>
   </si>
   <si>
     <t>btree_ps_batch_001</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>10000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select count(*) from $schema26 where id&gt;2000 and id&lt;=10000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>8000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>update $schema26 set name='BJ' where id&gt;2000 and id&lt;=10000</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -534,7 +534,7 @@
   <dimension ref="A1:W2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O2" sqref="O2"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -630,10 +630,10 @@
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A2" s="6" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>10</v>
@@ -648,7 +648,7 @@
         <v>31</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="J2" s="2" t="s">
         <v>32</v>
@@ -657,31 +657,31 @@
         <v>12</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="Q2" s="2" t="s">
         <v>22</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="S2" s="2" t="s">
         <v>25</v>
       </c>
       <c r="T2" s="2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="U2" s="2" t="s">
         <v>12</v>

</xml_diff>